<commit_message>
Removed After class tests
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1253,9 +1253,7 @@
       <c r="H3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added notification OR properties
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_JS.xlsx
@@ -427,41 +427,6 @@
 </t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
-SelectTestToRun(VT200_0009_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-Lock_UnlockScreen(lock);
-wait(2);
-Lock_UnlockScreen(unlock);
-wait(2);
-link_Click(stopCallback_name_xpath);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
-SelectTestToRun(VT200_0013_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(8);
-Lock_UnlockScreen(lock);
-wait(2);
-Lock_UnlockScreen(unlock);
-link_Click(stopCallback_name_xpath);
-wait(2);
-validate6;</t>
-  </si>
-  <si>
     <t xml:space="preserve">wait(5);
 validate1;
 link_Click(Application_test_link);
@@ -632,6 +597,39 @@
 validate1;
 link_Click(Application_test_link);
 validate2;
+SelectTestToRun(VT200_0009_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+Lock_UnlockScreen(lock);
+Lock_UnlockScreen(unlock);
+wait(2);
+link_Click(stopCallback_name_xpath);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(Application_test_link);
+validate2;
+SelectTestToRun(VT200_0013_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(8);
+Lock_UnlockScreen(lock);
+Lock_UnlockScreen(unlock);
+link_Click(stopCallback_name_xpath);
+wait(2);
+validate6;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(Application_test_link);
+validate2;
 SelectTestToRun(VT200_0012_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -639,9 +637,8 @@
 wait(2);
 launch_App_Device(com.android.browser/com.android.browser.BrowserActivity);
 Lock_UnlockScreen(lock);
-wait(2);
 Lock_UnlockScreen(unlock);
-launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
+press_Key(Back);
 validate4;
 link_Click(stopCallback_name_xpath);
 wait(2);
@@ -658,9 +655,8 @@
 ClickRunTest(runtest_bottom_xpath);
 wait(2);
 launch_App_Device(com.android.browser/com.android.browser.BrowserActivity);
-launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
+press_Key(Back);
 Lock_UnlockScreen(lock);
-wait(2);
 Lock_UnlockScreen(unlock);
 wait(2);
 link_Click(stopCallback_name_xpath);
@@ -1152,7 +1148,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1160,7 +1156,7 @@
     <col min="1" max="1" width="11.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="37.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1356,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>78</v>
@@ -1377,16 +1373,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1404,7 +1400,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1413,7 +1409,7 @@
         <v>93</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1437,16 +1433,16 @@
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="281.25" thickBot="1">
+    <row r="11" spans="1:11" ht="255.75" thickBot="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1467,7 +1463,7 @@
         <v>94</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1491,10 +1487,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1516,10 +1512,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="86.25" thickBot="1">

</xml_diff>